<commit_message>
adding options to ex141     bug fixed: market close candle is now ok
</commit_message>
<xml_diff>
--- a/reports/report.xlsx
+++ b/reports/report.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmral\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAMiD\AppData\Roaming\MetaQuotes\Terminal\36A64B8C79A6163D85E6173B54096685\MQL5\Experts\mq5ea\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F05142D0-0480-4904-BE1C-C5C309019E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44ABE334-4B72-44A6-83FF-66F8F1975958}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -553,44 +552,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEE0728-66BF-4A8D-AE3D-76DFDC44DA79}">
-  <dimension ref="A1:AF1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="18.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="13.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,31 +659,31 @@
       <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>